<commit_message>
Fixed dropping of index column.
</commit_message>
<xml_diff>
--- a/temp/final_output.xlsx
+++ b/temp/final_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F271"/>
+  <dimension ref="A1:E271"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,17 +451,12 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>CREDIT</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>DEBIT</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>CREDIT</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>original_index</t>
         </is>
       </c>
     </row>
@@ -481,9 +476,6 @@
       <c r="E2" t="n">
         <v>0</v>
       </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -501,9 +493,6 @@
       <c r="E3" t="n">
         <v>0</v>
       </c>
-      <c r="F3" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -518,13 +507,10 @@
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
         <v>19032106.67</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -540,13 +526,10 @@
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
         <v>1016.62</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -562,13 +545,10 @@
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
         <v>5000000</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -584,13 +564,10 @@
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
         <v>5000000</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="8">
@@ -606,13 +583,10 @@
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
         <v>5000000</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" t="n">
-        <v>6</v>
       </c>
     </row>
     <row r="9">
@@ -628,13 +602,10 @@
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
         <v>5000000</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="n">
-        <v>7</v>
       </c>
     </row>
     <row r="10">
@@ -650,13 +621,10 @@
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
         <v>5000000</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" t="n">
-        <v>8</v>
       </c>
     </row>
     <row r="11">
@@ -672,13 +640,10 @@
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
         <v>1123643.82</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
-        <v>9</v>
       </c>
     </row>
     <row r="12">
@@ -694,13 +659,10 @@
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
         <v>5000000</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" t="n">
-        <v>10</v>
       </c>
     </row>
     <row r="13">
@@ -716,13 +678,10 @@
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
         <v>5000000</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" t="n">
-        <v>11</v>
       </c>
     </row>
     <row r="14">
@@ -738,13 +697,10 @@
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
         <v>5000000</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" t="n">
-        <v>12</v>
       </c>
     </row>
     <row r="15">
@@ -760,13 +716,10 @@
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
         <v>5000000</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" t="n">
-        <v>13</v>
       </c>
     </row>
     <row r="16">
@@ -782,13 +735,10 @@
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
         <v>500</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" t="n">
-        <v>14</v>
       </c>
     </row>
     <row r="17">
@@ -804,13 +754,10 @@
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
         <v>899300</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" t="n">
-        <v>15</v>
       </c>
     </row>
     <row r="18">
@@ -826,13 +773,10 @@
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
         <v>403.65</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" t="n">
-        <v>16</v>
       </c>
     </row>
     <row r="19">
@@ -848,13 +792,10 @@
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
         <v>1000000</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" t="n">
-        <v>17</v>
       </c>
     </row>
     <row r="20">
@@ -870,13 +811,10 @@
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
         <v>5000000</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" t="n">
-        <v>18</v>
       </c>
     </row>
     <row r="21">
@@ -892,13 +830,10 @@
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
         <v>5000000</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" t="n">
-        <v>19</v>
       </c>
     </row>
     <row r="22">
@@ -914,13 +849,10 @@
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
         <v>5000000</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" t="n">
-        <v>20</v>
       </c>
     </row>
     <row r="23">
@@ -936,13 +868,10 @@
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
         <v>7157659.81</v>
-      </c>
-      <c r="E23" t="n">
-        <v>0</v>
-      </c>
-      <c r="F23" t="n">
-        <v>21</v>
       </c>
     </row>
     <row r="24">
@@ -958,13 +887,10 @@
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
         <v>7854860.74</v>
-      </c>
-      <c r="E24" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" t="n">
-        <v>22</v>
       </c>
     </row>
     <row r="25">
@@ -980,13 +906,10 @@
       </c>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="n">
         <v>11120082.01</v>
-      </c>
-      <c r="E25" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" t="n">
-        <v>23</v>
       </c>
     </row>
     <row r="26">
@@ -1002,13 +925,10 @@
       </c>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="n">
         <v>15203994.36</v>
-      </c>
-      <c r="E26" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" t="n">
-        <v>24</v>
       </c>
     </row>
     <row r="27">
@@ -1024,13 +944,10 @@
       </c>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="n">
         <v>34001556.05</v>
-      </c>
-      <c r="E27" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" t="n">
-        <v>25</v>
       </c>
     </row>
     <row r="28">
@@ -1050,13 +967,10 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>560.27</v>
       </c>
       <c r="E28" t="n">
-        <v>560.27</v>
-      </c>
-      <c r="F28" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1076,13 +990,10 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>712.51</v>
       </c>
       <c r="E29" t="n">
-        <v>712.51</v>
-      </c>
-      <c r="F29" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1098,13 +1009,10 @@
       </c>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="n">
-        <v>0</v>
+        <v>800</v>
       </c>
       <c r="E30" t="n">
-        <v>800</v>
-      </c>
-      <c r="F30" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -1124,13 +1032,10 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>0</v>
+        <v>825.41</v>
       </c>
       <c r="E31" t="n">
-        <v>825.41</v>
-      </c>
-      <c r="F31" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -1150,13 +1055,10 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>1506.05</v>
       </c>
       <c r="E32" t="n">
-        <v>1506.05</v>
-      </c>
-      <c r="F32" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1176,13 +1078,10 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>1676.12</v>
       </c>
       <c r="E33" t="n">
-        <v>1676.12</v>
-      </c>
-      <c r="F33" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -1202,13 +1101,10 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>1839.27</v>
       </c>
       <c r="E34" t="n">
-        <v>1839.27</v>
-      </c>
-      <c r="F34" t="n">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -1228,13 +1124,10 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>0</v>
+        <v>2185</v>
       </c>
       <c r="E35" t="n">
-        <v>2185</v>
-      </c>
-      <c r="F35" t="n">
-        <v>33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -1254,13 +1147,10 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>2359.76</v>
       </c>
       <c r="E36" t="n">
-        <v>2359.76</v>
-      </c>
-      <c r="F36" t="n">
-        <v>34</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -1280,13 +1170,10 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>2468.72</v>
       </c>
       <c r="E37" t="n">
-        <v>2468.72</v>
-      </c>
-      <c r="F37" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -1306,13 +1193,10 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0</v>
+        <v>2663.46</v>
       </c>
       <c r="E38" t="n">
-        <v>2663.46</v>
-      </c>
-      <c r="F38" t="n">
-        <v>36</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -1328,13 +1212,10 @@
       </c>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="n">
-        <v>0</v>
+        <v>2754</v>
       </c>
       <c r="E39" t="n">
-        <v>2754</v>
-      </c>
-      <c r="F39" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -1354,13 +1235,10 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0</v>
+        <v>3030.65</v>
       </c>
       <c r="E40" t="n">
-        <v>3030.65</v>
-      </c>
-      <c r="F40" t="n">
-        <v>38</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -1380,13 +1258,10 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0</v>
+        <v>3099.38</v>
       </c>
       <c r="E41" t="n">
-        <v>3099.38</v>
-      </c>
-      <c r="F41" t="n">
-        <v>39</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -1406,13 +1281,10 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0</v>
+        <v>3150</v>
       </c>
       <c r="E42" t="n">
-        <v>3150</v>
-      </c>
-      <c r="F42" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -1432,13 +1304,10 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0</v>
+        <v>3200.37</v>
       </c>
       <c r="E43" t="n">
-        <v>3200.37</v>
-      </c>
-      <c r="F43" t="n">
-        <v>41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -1458,13 +1327,10 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0</v>
+        <v>3209.51</v>
       </c>
       <c r="E44" t="n">
-        <v>3209.51</v>
-      </c>
-      <c r="F44" t="n">
-        <v>42</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -1484,13 +1350,10 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>0</v>
+        <v>3214.8</v>
       </c>
       <c r="E45" t="n">
-        <v>3214.8</v>
-      </c>
-      <c r="F45" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -1510,13 +1373,10 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>0</v>
+        <v>3234.38</v>
       </c>
       <c r="E46" t="n">
-        <v>3234.38</v>
-      </c>
-      <c r="F46" t="n">
-        <v>44</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -1536,13 +1396,10 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>0</v>
+        <v>3268.91</v>
       </c>
       <c r="E47" t="n">
-        <v>3268.91</v>
-      </c>
-      <c r="F47" t="n">
-        <v>45</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -1562,13 +1419,10 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>0</v>
+        <v>3370.7</v>
       </c>
       <c r="E48" t="n">
-        <v>3370.7</v>
-      </c>
-      <c r="F48" t="n">
-        <v>46</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -1584,13 +1438,10 @@
       </c>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="n">
-        <v>0</v>
+        <v>3512.44</v>
       </c>
       <c r="E49" t="n">
-        <v>3512.44</v>
-      </c>
-      <c r="F49" t="n">
-        <v>47</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -1610,13 +1461,10 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0</v>
+        <v>3813.72</v>
       </c>
       <c r="E50" t="n">
-        <v>3813.72</v>
-      </c>
-      <c r="F50" t="n">
-        <v>48</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -1636,13 +1484,10 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0</v>
+        <v>4104</v>
       </c>
       <c r="E51" t="n">
-        <v>4104</v>
-      </c>
-      <c r="F51" t="n">
-        <v>49</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -1662,13 +1507,10 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>0</v>
+        <v>4306.81</v>
       </c>
       <c r="E52" t="n">
-        <v>4306.81</v>
-      </c>
-      <c r="F52" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -1688,13 +1530,10 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>0</v>
+        <v>4311.14</v>
       </c>
       <c r="E53" t="n">
-        <v>4311.14</v>
-      </c>
-      <c r="F53" t="n">
-        <v>51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -1714,13 +1553,10 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>0</v>
+        <v>4400</v>
       </c>
       <c r="E54" t="n">
-        <v>4400</v>
-      </c>
-      <c r="F54" t="n">
-        <v>52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -1736,13 +1572,10 @@
       </c>
       <c r="C55" t="inlineStr"/>
       <c r="D55" t="n">
-        <v>0</v>
+        <v>4645.17</v>
       </c>
       <c r="E55" t="n">
-        <v>4645.17</v>
-      </c>
-      <c r="F55" t="n">
-        <v>53</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -1762,13 +1595,10 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>0</v>
+        <v>5340.61</v>
       </c>
       <c r="E56" t="n">
-        <v>5340.61</v>
-      </c>
-      <c r="F56" t="n">
-        <v>54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -1788,13 +1618,10 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>0</v>
+        <v>5558.62</v>
       </c>
       <c r="E57" t="n">
-        <v>5558.62</v>
-      </c>
-      <c r="F57" t="n">
-        <v>55</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -1814,13 +1641,10 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>0</v>
+        <v>5877.65</v>
       </c>
       <c r="E58" t="n">
-        <v>5877.65</v>
-      </c>
-      <c r="F58" t="n">
-        <v>56</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -1840,13 +1664,10 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>0</v>
+        <v>5997.83</v>
       </c>
       <c r="E59" t="n">
-        <v>5997.83</v>
-      </c>
-      <c r="F59" t="n">
-        <v>57</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -1862,13 +1683,10 @@
       </c>
       <c r="C60" t="inlineStr"/>
       <c r="D60" t="n">
-        <v>0</v>
+        <v>6142.54</v>
       </c>
       <c r="E60" t="n">
-        <v>6142.54</v>
-      </c>
-      <c r="F60" t="n">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -1884,13 +1702,10 @@
       </c>
       <c r="C61" t="inlineStr"/>
       <c r="D61" t="n">
-        <v>0</v>
+        <v>6285.48</v>
       </c>
       <c r="E61" t="n">
-        <v>6285.48</v>
-      </c>
-      <c r="F61" t="n">
-        <v>59</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -1910,13 +1725,10 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>0</v>
+        <v>6405.45</v>
       </c>
       <c r="E62" t="n">
-        <v>6405.45</v>
-      </c>
-      <c r="F62" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -1936,13 +1748,10 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>0</v>
+        <v>6532.03</v>
       </c>
       <c r="E63" t="n">
-        <v>6532.03</v>
-      </c>
-      <c r="F63" t="n">
-        <v>61</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -1962,13 +1771,10 @@
         </is>
       </c>
       <c r="D64" t="n">
-        <v>0</v>
+        <v>6610</v>
       </c>
       <c r="E64" t="n">
-        <v>6610</v>
-      </c>
-      <c r="F64" t="n">
-        <v>62</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -1988,13 +1794,10 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>0</v>
+        <v>7156.07</v>
       </c>
       <c r="E65" t="n">
-        <v>7156.07</v>
-      </c>
-      <c r="F65" t="n">
-        <v>63</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -2014,13 +1817,10 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>0</v>
+        <v>7489.82</v>
       </c>
       <c r="E66" t="n">
-        <v>7489.82</v>
-      </c>
-      <c r="F66" t="n">
-        <v>64</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -2040,13 +1840,10 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>0</v>
+        <v>7533.49</v>
       </c>
       <c r="E67" t="n">
-        <v>7533.49</v>
-      </c>
-      <c r="F67" t="n">
-        <v>65</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -2066,13 +1863,10 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>0</v>
+        <v>7670.7</v>
       </c>
       <c r="E68" t="n">
-        <v>7670.7</v>
-      </c>
-      <c r="F68" t="n">
-        <v>66</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -2092,13 +1886,10 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>0</v>
+        <v>8788.85</v>
       </c>
       <c r="E69" t="n">
-        <v>8788.85</v>
-      </c>
-      <c r="F69" t="n">
-        <v>67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -2118,13 +1909,10 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>0</v>
+        <v>8863.360000000001</v>
       </c>
       <c r="E70" t="n">
-        <v>8863.360000000001</v>
-      </c>
-      <c r="F70" t="n">
-        <v>68</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -2144,13 +1932,10 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>0</v>
+        <v>8897.700000000001</v>
       </c>
       <c r="E71" t="n">
-        <v>8897.700000000001</v>
-      </c>
-      <c r="F71" t="n">
-        <v>69</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -2170,13 +1955,10 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>0</v>
+        <v>8910</v>
       </c>
       <c r="E72" t="n">
-        <v>8910</v>
-      </c>
-      <c r="F72" t="n">
-        <v>70</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -2196,13 +1978,10 @@
         </is>
       </c>
       <c r="D73" t="n">
-        <v>0</v>
+        <v>8948.719999999999</v>
       </c>
       <c r="E73" t="n">
-        <v>8948.719999999999</v>
-      </c>
-      <c r="F73" t="n">
-        <v>71</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -2222,13 +2001,10 @@
         </is>
       </c>
       <c r="D74" t="n">
-        <v>0</v>
+        <v>9306.370000000001</v>
       </c>
       <c r="E74" t="n">
-        <v>9306.370000000001</v>
-      </c>
-      <c r="F74" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -2244,13 +2020,10 @@
       </c>
       <c r="C75" t="inlineStr"/>
       <c r="D75" t="n">
-        <v>0</v>
+        <v>9499</v>
       </c>
       <c r="E75" t="n">
-        <v>9499</v>
-      </c>
-      <c r="F75" t="n">
-        <v>73</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -2270,13 +2043,10 @@
         </is>
       </c>
       <c r="D76" t="n">
-        <v>0</v>
+        <v>9598.5</v>
       </c>
       <c r="E76" t="n">
-        <v>9598.5</v>
-      </c>
-      <c r="F76" t="n">
-        <v>74</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -2296,13 +2066,10 @@
         </is>
       </c>
       <c r="D77" t="n">
-        <v>0</v>
+        <v>9672.75</v>
       </c>
       <c r="E77" t="n">
-        <v>9672.75</v>
-      </c>
-      <c r="F77" t="n">
-        <v>75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -2322,13 +2089,10 @@
         </is>
       </c>
       <c r="D78" t="n">
-        <v>0</v>
+        <v>9715.66</v>
       </c>
       <c r="E78" t="n">
-        <v>9715.66</v>
-      </c>
-      <c r="F78" t="n">
-        <v>76</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -2344,13 +2108,10 @@
       </c>
       <c r="C79" t="inlineStr"/>
       <c r="D79" t="n">
-        <v>0</v>
+        <v>10255</v>
       </c>
       <c r="E79" t="n">
-        <v>10255</v>
-      </c>
-      <c r="F79" t="n">
-        <v>77</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80">
@@ -2370,13 +2131,10 @@
         </is>
       </c>
       <c r="D80" t="n">
-        <v>0</v>
+        <v>10971</v>
       </c>
       <c r="E80" t="n">
-        <v>10971</v>
-      </c>
-      <c r="F80" t="n">
-        <v>78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -2396,13 +2154,10 @@
         </is>
       </c>
       <c r="D81" t="n">
-        <v>0</v>
+        <v>11673.45</v>
       </c>
       <c r="E81" t="n">
-        <v>11673.45</v>
-      </c>
-      <c r="F81" t="n">
-        <v>79</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -2422,13 +2177,10 @@
         </is>
       </c>
       <c r="D82" t="n">
-        <v>0</v>
+        <v>11952</v>
       </c>
       <c r="E82" t="n">
-        <v>11952</v>
-      </c>
-      <c r="F82" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -2448,13 +2200,10 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>0</v>
+        <v>12066.8</v>
       </c>
       <c r="E83" t="n">
-        <v>12066.8</v>
-      </c>
-      <c r="F83" t="n">
-        <v>81</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -2474,13 +2223,10 @@
         </is>
       </c>
       <c r="D84" t="n">
-        <v>0</v>
+        <v>12898.72</v>
       </c>
       <c r="E84" t="n">
-        <v>12898.72</v>
-      </c>
-      <c r="F84" t="n">
-        <v>82</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -2500,13 +2246,10 @@
         </is>
       </c>
       <c r="D85" t="n">
-        <v>0</v>
+        <v>13055.37</v>
       </c>
       <c r="E85" t="n">
-        <v>13055.37</v>
-      </c>
-      <c r="F85" t="n">
-        <v>83</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -2526,13 +2269,10 @@
         </is>
       </c>
       <c r="D86" t="n">
-        <v>0</v>
+        <v>13092.17</v>
       </c>
       <c r="E86" t="n">
-        <v>13092.17</v>
-      </c>
-      <c r="F86" t="n">
-        <v>84</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -2552,13 +2292,10 @@
         </is>
       </c>
       <c r="D87" t="n">
-        <v>0</v>
+        <v>13190.43</v>
       </c>
       <c r="E87" t="n">
-        <v>13190.43</v>
-      </c>
-      <c r="F87" t="n">
-        <v>85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88">
@@ -2578,13 +2315,10 @@
         </is>
       </c>
       <c r="D88" t="n">
-        <v>0</v>
+        <v>13370.91</v>
       </c>
       <c r="E88" t="n">
-        <v>13370.91</v>
-      </c>
-      <c r="F88" t="n">
-        <v>86</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89">
@@ -2604,13 +2338,10 @@
         </is>
       </c>
       <c r="D89" t="n">
-        <v>0</v>
+        <v>13458.24</v>
       </c>
       <c r="E89" t="n">
-        <v>13458.24</v>
-      </c>
-      <c r="F89" t="n">
-        <v>87</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90">
@@ -2630,13 +2361,10 @@
         </is>
       </c>
       <c r="D90" t="n">
-        <v>0</v>
+        <v>13665.75</v>
       </c>
       <c r="E90" t="n">
-        <v>13665.75</v>
-      </c>
-      <c r="F90" t="n">
-        <v>88</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -2656,13 +2384,10 @@
         </is>
       </c>
       <c r="D91" t="n">
-        <v>0</v>
+        <v>13948.95</v>
       </c>
       <c r="E91" t="n">
-        <v>13948.95</v>
-      </c>
-      <c r="F91" t="n">
-        <v>89</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92">
@@ -2682,13 +2407,10 @@
         </is>
       </c>
       <c r="D92" t="n">
-        <v>0</v>
+        <v>13982.99</v>
       </c>
       <c r="E92" t="n">
-        <v>13982.99</v>
-      </c>
-      <c r="F92" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93">
@@ -2708,13 +2430,10 @@
         </is>
       </c>
       <c r="D93" t="n">
-        <v>0</v>
+        <v>14016.38</v>
       </c>
       <c r="E93" t="n">
-        <v>14016.38</v>
-      </c>
-      <c r="F93" t="n">
-        <v>91</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94">
@@ -2734,13 +2453,10 @@
         </is>
       </c>
       <c r="D94" t="n">
-        <v>0</v>
+        <v>14278.4</v>
       </c>
       <c r="E94" t="n">
-        <v>14278.4</v>
-      </c>
-      <c r="F94" t="n">
-        <v>92</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95">
@@ -2760,13 +2476,10 @@
         </is>
       </c>
       <c r="D95" t="n">
-        <v>0</v>
+        <v>14491.92</v>
       </c>
       <c r="E95" t="n">
-        <v>14491.92</v>
-      </c>
-      <c r="F95" t="n">
-        <v>93</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96">
@@ -2786,13 +2499,10 @@
         </is>
       </c>
       <c r="D96" t="n">
-        <v>0</v>
+        <v>14722.88</v>
       </c>
       <c r="E96" t="n">
-        <v>14722.88</v>
-      </c>
-      <c r="F96" t="n">
-        <v>94</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97">
@@ -2812,13 +2522,10 @@
         </is>
       </c>
       <c r="D97" t="n">
-        <v>0</v>
+        <v>14974.77</v>
       </c>
       <c r="E97" t="n">
-        <v>14974.77</v>
-      </c>
-      <c r="F97" t="n">
-        <v>95</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98">
@@ -2838,13 +2545,10 @@
         </is>
       </c>
       <c r="D98" t="n">
-        <v>0</v>
+        <v>15500</v>
       </c>
       <c r="E98" t="n">
-        <v>15500</v>
-      </c>
-      <c r="F98" t="n">
-        <v>96</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99">
@@ -2864,13 +2568,10 @@
         </is>
       </c>
       <c r="D99" t="n">
-        <v>0</v>
+        <v>15532.12</v>
       </c>
       <c r="E99" t="n">
-        <v>15532.12</v>
-      </c>
-      <c r="F99" t="n">
-        <v>97</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100">
@@ -2890,13 +2591,10 @@
         </is>
       </c>
       <c r="D100" t="n">
-        <v>0</v>
+        <v>15624</v>
       </c>
       <c r="E100" t="n">
-        <v>15624</v>
-      </c>
-      <c r="F100" t="n">
-        <v>98</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101">
@@ -2916,13 +2614,10 @@
         </is>
       </c>
       <c r="D101" t="n">
-        <v>0</v>
+        <v>15653.61</v>
       </c>
       <c r="E101" t="n">
-        <v>15653.61</v>
-      </c>
-      <c r="F101" t="n">
-        <v>99</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102">
@@ -2942,13 +2637,10 @@
         </is>
       </c>
       <c r="D102" t="n">
-        <v>0</v>
+        <v>15784.38</v>
       </c>
       <c r="E102" t="n">
-        <v>15784.38</v>
-      </c>
-      <c r="F102" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103">
@@ -2968,13 +2660,10 @@
         </is>
       </c>
       <c r="D103" t="n">
-        <v>0</v>
+        <v>15989.59</v>
       </c>
       <c r="E103" t="n">
-        <v>15989.59</v>
-      </c>
-      <c r="F103" t="n">
-        <v>101</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104">
@@ -2994,13 +2683,10 @@
         </is>
       </c>
       <c r="D104" t="n">
-        <v>0</v>
+        <v>16053</v>
       </c>
       <c r="E104" t="n">
-        <v>16053</v>
-      </c>
-      <c r="F104" t="n">
-        <v>102</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105">
@@ -3016,13 +2702,10 @@
       </c>
       <c r="C105" t="inlineStr"/>
       <c r="D105" t="n">
-        <v>0</v>
+        <v>16145.83</v>
       </c>
       <c r="E105" t="n">
-        <v>16145.83</v>
-      </c>
-      <c r="F105" t="n">
-        <v>103</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106">
@@ -3042,13 +2725,10 @@
         </is>
       </c>
       <c r="D106" t="n">
-        <v>0</v>
+        <v>16781.62</v>
       </c>
       <c r="E106" t="n">
-        <v>16781.62</v>
-      </c>
-      <c r="F106" t="n">
-        <v>104</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107">
@@ -3068,13 +2748,10 @@
         </is>
       </c>
       <c r="D107" t="n">
-        <v>0</v>
+        <v>17030.55</v>
       </c>
       <c r="E107" t="n">
-        <v>17030.55</v>
-      </c>
-      <c r="F107" t="n">
-        <v>105</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108">
@@ -3094,13 +2771,10 @@
         </is>
       </c>
       <c r="D108" t="n">
-        <v>0</v>
+        <v>17033.04</v>
       </c>
       <c r="E108" t="n">
-        <v>17033.04</v>
-      </c>
-      <c r="F108" t="n">
-        <v>106</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109">
@@ -3120,13 +2794,10 @@
         </is>
       </c>
       <c r="D109" t="n">
-        <v>0</v>
+        <v>17058.96</v>
       </c>
       <c r="E109" t="n">
-        <v>17058.96</v>
-      </c>
-      <c r="F109" t="n">
-        <v>107</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110">
@@ -3146,13 +2817,10 @@
         </is>
       </c>
       <c r="D110" t="n">
-        <v>0</v>
+        <v>17983.13</v>
       </c>
       <c r="E110" t="n">
-        <v>17983.13</v>
-      </c>
-      <c r="F110" t="n">
-        <v>108</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111">
@@ -3172,13 +2840,10 @@
         </is>
       </c>
       <c r="D111" t="n">
-        <v>0</v>
+        <v>18115.71</v>
       </c>
       <c r="E111" t="n">
-        <v>18115.71</v>
-      </c>
-      <c r="F111" t="n">
-        <v>109</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112">
@@ -3194,13 +2859,10 @@
       </c>
       <c r="C112" t="inlineStr"/>
       <c r="D112" t="n">
-        <v>0</v>
+        <v>19120.61</v>
       </c>
       <c r="E112" t="n">
-        <v>19120.61</v>
-      </c>
-      <c r="F112" t="n">
-        <v>110</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113">
@@ -3220,13 +2882,10 @@
         </is>
       </c>
       <c r="D113" t="n">
-        <v>0</v>
+        <v>19438.68</v>
       </c>
       <c r="E113" t="n">
-        <v>19438.68</v>
-      </c>
-      <c r="F113" t="n">
-        <v>111</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114">
@@ -3246,13 +2905,10 @@
         </is>
       </c>
       <c r="D114" t="n">
-        <v>0</v>
+        <v>20786.48</v>
       </c>
       <c r="E114" t="n">
-        <v>20786.48</v>
-      </c>
-      <c r="F114" t="n">
-        <v>112</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115">
@@ -3272,13 +2928,10 @@
         </is>
       </c>
       <c r="D115" t="n">
-        <v>0</v>
+        <v>20841.32</v>
       </c>
       <c r="E115" t="n">
-        <v>20841.32</v>
-      </c>
-      <c r="F115" t="n">
-        <v>113</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116">
@@ -3298,13 +2951,10 @@
         </is>
       </c>
       <c r="D116" t="n">
-        <v>0</v>
+        <v>21258.78</v>
       </c>
       <c r="E116" t="n">
-        <v>21258.78</v>
-      </c>
-      <c r="F116" t="n">
-        <v>114</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117">
@@ -3324,13 +2974,10 @@
         </is>
       </c>
       <c r="D117" t="n">
-        <v>0</v>
+        <v>21412.36</v>
       </c>
       <c r="E117" t="n">
-        <v>21412.36</v>
-      </c>
-      <c r="F117" t="n">
-        <v>115</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118">
@@ -3350,13 +2997,10 @@
         </is>
       </c>
       <c r="D118" t="n">
-        <v>0</v>
+        <v>21871.67</v>
       </c>
       <c r="E118" t="n">
-        <v>21871.67</v>
-      </c>
-      <c r="F118" t="n">
-        <v>116</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119">
@@ -3376,13 +3020,10 @@
         </is>
       </c>
       <c r="D119" t="n">
-        <v>0</v>
+        <v>22086.9</v>
       </c>
       <c r="E119" t="n">
-        <v>22086.9</v>
-      </c>
-      <c r="F119" t="n">
-        <v>117</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120">
@@ -3402,13 +3043,10 @@
         </is>
       </c>
       <c r="D120" t="n">
-        <v>0</v>
+        <v>22449.87</v>
       </c>
       <c r="E120" t="n">
-        <v>22449.87</v>
-      </c>
-      <c r="F120" t="n">
-        <v>118</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121">
@@ -3428,13 +3066,10 @@
         </is>
       </c>
       <c r="D121" t="n">
-        <v>0</v>
+        <v>22980.87</v>
       </c>
       <c r="E121" t="n">
-        <v>22980.87</v>
-      </c>
-      <c r="F121" t="n">
-        <v>119</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122">
@@ -3454,13 +3089,10 @@
         </is>
       </c>
       <c r="D122" t="n">
-        <v>0</v>
+        <v>23421.39</v>
       </c>
       <c r="E122" t="n">
-        <v>23421.39</v>
-      </c>
-      <c r="F122" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123">
@@ -3480,13 +3112,10 @@
         </is>
       </c>
       <c r="D123" t="n">
-        <v>0</v>
+        <v>24729.83</v>
       </c>
       <c r="E123" t="n">
-        <v>24729.83</v>
-      </c>
-      <c r="F123" t="n">
-        <v>121</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124">
@@ -3506,13 +3135,10 @@
         </is>
       </c>
       <c r="D124" t="n">
-        <v>0</v>
+        <v>24992.64</v>
       </c>
       <c r="E124" t="n">
-        <v>24992.64</v>
-      </c>
-      <c r="F124" t="n">
-        <v>122</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125">
@@ -3532,13 +3158,10 @@
         </is>
       </c>
       <c r="D125" t="n">
-        <v>0</v>
+        <v>25354.97</v>
       </c>
       <c r="E125" t="n">
-        <v>25354.97</v>
-      </c>
-      <c r="F125" t="n">
-        <v>123</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126">
@@ -3558,13 +3181,10 @@
         </is>
       </c>
       <c r="D126" t="n">
-        <v>0</v>
+        <v>26235.06</v>
       </c>
       <c r="E126" t="n">
-        <v>26235.06</v>
-      </c>
-      <c r="F126" t="n">
-        <v>124</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127">
@@ -3584,13 +3204,10 @@
         </is>
       </c>
       <c r="D127" t="n">
-        <v>0</v>
+        <v>26581.95</v>
       </c>
       <c r="E127" t="n">
-        <v>26581.95</v>
-      </c>
-      <c r="F127" t="n">
-        <v>125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128">
@@ -3610,13 +3227,10 @@
         </is>
       </c>
       <c r="D128" t="n">
-        <v>0</v>
+        <v>27324</v>
       </c>
       <c r="E128" t="n">
-        <v>27324</v>
-      </c>
-      <c r="F128" t="n">
-        <v>126</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129">
@@ -3636,13 +3250,10 @@
         </is>
       </c>
       <c r="D129" t="n">
-        <v>0</v>
+        <v>27777.74</v>
       </c>
       <c r="E129" t="n">
-        <v>27777.74</v>
-      </c>
-      <c r="F129" t="n">
-        <v>127</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130">
@@ -3662,13 +3273,10 @@
         </is>
       </c>
       <c r="D130" t="n">
-        <v>0</v>
+        <v>27896.96</v>
       </c>
       <c r="E130" t="n">
-        <v>27896.96</v>
-      </c>
-      <c r="F130" t="n">
-        <v>128</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131">
@@ -3688,13 +3296,10 @@
         </is>
       </c>
       <c r="D131" t="n">
-        <v>0</v>
+        <v>28025.21</v>
       </c>
       <c r="E131" t="n">
-        <v>28025.21</v>
-      </c>
-      <c r="F131" t="n">
-        <v>129</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132">
@@ -3714,13 +3319,10 @@
         </is>
       </c>
       <c r="D132" t="n">
-        <v>0</v>
+        <v>28100.66</v>
       </c>
       <c r="E132" t="n">
-        <v>28100.66</v>
-      </c>
-      <c r="F132" t="n">
-        <v>130</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133">
@@ -3740,13 +3342,10 @@
         </is>
       </c>
       <c r="D133" t="n">
-        <v>0</v>
+        <v>28527.19</v>
       </c>
       <c r="E133" t="n">
-        <v>28527.19</v>
-      </c>
-      <c r="F133" t="n">
-        <v>131</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134">
@@ -3762,13 +3361,10 @@
       </c>
       <c r="C134" t="inlineStr"/>
       <c r="D134" t="n">
-        <v>0</v>
+        <v>28757.7</v>
       </c>
       <c r="E134" t="n">
-        <v>28757.7</v>
-      </c>
-      <c r="F134" t="n">
-        <v>132</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135">
@@ -3788,13 +3384,10 @@
         </is>
       </c>
       <c r="D135" t="n">
-        <v>0</v>
+        <v>28933.84</v>
       </c>
       <c r="E135" t="n">
-        <v>28933.84</v>
-      </c>
-      <c r="F135" t="n">
-        <v>133</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136">
@@ -3810,13 +3403,10 @@
       </c>
       <c r="C136" t="inlineStr"/>
       <c r="D136" t="n">
-        <v>0</v>
+        <v>29389.77</v>
       </c>
       <c r="E136" t="n">
-        <v>29389.77</v>
-      </c>
-      <c r="F136" t="n">
-        <v>134</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137">
@@ -3836,13 +3426,10 @@
         </is>
       </c>
       <c r="D137" t="n">
-        <v>0</v>
+        <v>30515.93</v>
       </c>
       <c r="E137" t="n">
-        <v>30515.93</v>
-      </c>
-      <c r="F137" t="n">
-        <v>135</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138">
@@ -3862,13 +3449,10 @@
         </is>
       </c>
       <c r="D138" t="n">
-        <v>0</v>
+        <v>31019.6</v>
       </c>
       <c r="E138" t="n">
-        <v>31019.6</v>
-      </c>
-      <c r="F138" t="n">
-        <v>136</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139">
@@ -3888,13 +3472,10 @@
         </is>
       </c>
       <c r="D139" t="n">
-        <v>0</v>
+        <v>31424.85</v>
       </c>
       <c r="E139" t="n">
-        <v>31424.85</v>
-      </c>
-      <c r="F139" t="n">
-        <v>137</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140">
@@ -3914,13 +3495,10 @@
         </is>
       </c>
       <c r="D140" t="n">
-        <v>0</v>
+        <v>31740.89</v>
       </c>
       <c r="E140" t="n">
-        <v>31740.89</v>
-      </c>
-      <c r="F140" t="n">
-        <v>138</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141">
@@ -3940,13 +3518,10 @@
         </is>
       </c>
       <c r="D141" t="n">
-        <v>0</v>
+        <v>32427.67</v>
       </c>
       <c r="E141" t="n">
-        <v>32427.67</v>
-      </c>
-      <c r="F141" t="n">
-        <v>139</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142">
@@ -3966,13 +3541,10 @@
         </is>
       </c>
       <c r="D142" t="n">
-        <v>0</v>
+        <v>32580</v>
       </c>
       <c r="E142" t="n">
-        <v>32580</v>
-      </c>
-      <c r="F142" t="n">
-        <v>140</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143">
@@ -3992,13 +3564,10 @@
         </is>
       </c>
       <c r="D143" t="n">
-        <v>0</v>
+        <v>33964.2</v>
       </c>
       <c r="E143" t="n">
-        <v>33964.2</v>
-      </c>
-      <c r="F143" t="n">
-        <v>141</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144">
@@ -4018,13 +3587,10 @@
         </is>
       </c>
       <c r="D144" t="n">
-        <v>0</v>
+        <v>34593.98</v>
       </c>
       <c r="E144" t="n">
-        <v>34593.98</v>
-      </c>
-      <c r="F144" t="n">
-        <v>142</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145">
@@ -4044,13 +3610,10 @@
         </is>
       </c>
       <c r="D145" t="n">
-        <v>0</v>
+        <v>34706.3</v>
       </c>
       <c r="E145" t="n">
-        <v>34706.3</v>
-      </c>
-      <c r="F145" t="n">
-        <v>143</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146">
@@ -4070,13 +3633,10 @@
         </is>
       </c>
       <c r="D146" t="n">
-        <v>0</v>
+        <v>34731.82</v>
       </c>
       <c r="E146" t="n">
-        <v>34731.82</v>
-      </c>
-      <c r="F146" t="n">
-        <v>144</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147">
@@ -4096,13 +3656,10 @@
         </is>
       </c>
       <c r="D147" t="n">
-        <v>0</v>
+        <v>34750</v>
       </c>
       <c r="E147" t="n">
-        <v>34750</v>
-      </c>
-      <c r="F147" t="n">
-        <v>145</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148">
@@ -4122,13 +3679,10 @@
         </is>
       </c>
       <c r="D148" t="n">
-        <v>0</v>
+        <v>35236.74</v>
       </c>
       <c r="E148" t="n">
-        <v>35236.74</v>
-      </c>
-      <c r="F148" t="n">
-        <v>146</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149">
@@ -4148,13 +3702,10 @@
         </is>
       </c>
       <c r="D149" t="n">
-        <v>0</v>
+        <v>35667.99</v>
       </c>
       <c r="E149" t="n">
-        <v>35667.99</v>
-      </c>
-      <c r="F149" t="n">
-        <v>147</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150">
@@ -4174,13 +3725,10 @@
         </is>
       </c>
       <c r="D150" t="n">
-        <v>0</v>
+        <v>38185.84</v>
       </c>
       <c r="E150" t="n">
-        <v>38185.84</v>
-      </c>
-      <c r="F150" t="n">
-        <v>148</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151">
@@ -4200,13 +3748,10 @@
         </is>
       </c>
       <c r="D151" t="n">
-        <v>0</v>
+        <v>40419.65</v>
       </c>
       <c r="E151" t="n">
-        <v>40419.65</v>
-      </c>
-      <c r="F151" t="n">
-        <v>149</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152">
@@ -4226,13 +3771,10 @@
         </is>
       </c>
       <c r="D152" t="n">
-        <v>0</v>
+        <v>40662.2</v>
       </c>
       <c r="E152" t="n">
-        <v>40662.2</v>
-      </c>
-      <c r="F152" t="n">
-        <v>150</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153">
@@ -4252,13 +3794,10 @@
         </is>
       </c>
       <c r="D153" t="n">
-        <v>0</v>
+        <v>42194.88</v>
       </c>
       <c r="E153" t="n">
-        <v>42194.88</v>
-      </c>
-      <c r="F153" t="n">
-        <v>151</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154">
@@ -4278,13 +3817,10 @@
         </is>
       </c>
       <c r="D154" t="n">
-        <v>0</v>
+        <v>42951.38</v>
       </c>
       <c r="E154" t="n">
-        <v>42951.38</v>
-      </c>
-      <c r="F154" t="n">
-        <v>152</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155">
@@ -4304,13 +3840,10 @@
         </is>
       </c>
       <c r="D155" t="n">
-        <v>0</v>
+        <v>43188.82</v>
       </c>
       <c r="E155" t="n">
-        <v>43188.82</v>
-      </c>
-      <c r="F155" t="n">
-        <v>153</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156">
@@ -4330,13 +3863,10 @@
         </is>
       </c>
       <c r="D156" t="n">
-        <v>0</v>
+        <v>43500.89</v>
       </c>
       <c r="E156" t="n">
-        <v>43500.89</v>
-      </c>
-      <c r="F156" t="n">
-        <v>154</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157">
@@ -4356,13 +3886,10 @@
         </is>
       </c>
       <c r="D157" t="n">
-        <v>0</v>
+        <v>43900</v>
       </c>
       <c r="E157" t="n">
-        <v>43900</v>
-      </c>
-      <c r="F157" t="n">
-        <v>155</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158">
@@ -4382,13 +3909,10 @@
         </is>
       </c>
       <c r="D158" t="n">
-        <v>0</v>
+        <v>45500.42</v>
       </c>
       <c r="E158" t="n">
-        <v>45500.42</v>
-      </c>
-      <c r="F158" t="n">
-        <v>156</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159">
@@ -4408,13 +3932,10 @@
         </is>
       </c>
       <c r="D159" t="n">
-        <v>0</v>
+        <v>45876.73</v>
       </c>
       <c r="E159" t="n">
-        <v>45876.73</v>
-      </c>
-      <c r="F159" t="n">
-        <v>157</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160">
@@ -4434,13 +3955,10 @@
         </is>
       </c>
       <c r="D160" t="n">
-        <v>0</v>
+        <v>46251</v>
       </c>
       <c r="E160" t="n">
-        <v>46251</v>
-      </c>
-      <c r="F160" t="n">
-        <v>158</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161">
@@ -4460,13 +3978,10 @@
         </is>
       </c>
       <c r="D161" t="n">
-        <v>0</v>
+        <v>47187.5</v>
       </c>
       <c r="E161" t="n">
-        <v>47187.5</v>
-      </c>
-      <c r="F161" t="n">
-        <v>159</v>
+        <v>0</v>
       </c>
     </row>
     <row r="162">
@@ -4486,13 +4001,10 @@
         </is>
       </c>
       <c r="D162" t="n">
-        <v>0</v>
+        <v>47474.93</v>
       </c>
       <c r="E162" t="n">
-        <v>47474.93</v>
-      </c>
-      <c r="F162" t="n">
-        <v>160</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163">
@@ -4508,13 +4020,10 @@
       </c>
       <c r="C163" t="inlineStr"/>
       <c r="D163" t="n">
-        <v>0</v>
+        <v>47639.06</v>
       </c>
       <c r="E163" t="n">
-        <v>47639.06</v>
-      </c>
-      <c r="F163" t="n">
-        <v>161</v>
+        <v>0</v>
       </c>
     </row>
     <row r="164">
@@ -4530,13 +4039,10 @@
       </c>
       <c r="C164" t="inlineStr"/>
       <c r="D164" t="n">
-        <v>0</v>
+        <v>47816.94</v>
       </c>
       <c r="E164" t="n">
-        <v>47816.94</v>
-      </c>
-      <c r="F164" t="n">
-        <v>162</v>
+        <v>0</v>
       </c>
     </row>
     <row r="165">
@@ -4556,13 +4062,10 @@
         </is>
       </c>
       <c r="D165" t="n">
-        <v>0</v>
+        <v>47899.61</v>
       </c>
       <c r="E165" t="n">
-        <v>47899.61</v>
-      </c>
-      <c r="F165" t="n">
-        <v>163</v>
+        <v>0</v>
       </c>
     </row>
     <row r="166">
@@ -4582,13 +4085,10 @@
         </is>
       </c>
       <c r="D166" t="n">
-        <v>0</v>
+        <v>48846.6</v>
       </c>
       <c r="E166" t="n">
-        <v>48846.6</v>
-      </c>
-      <c r="F166" t="n">
-        <v>164</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167">
@@ -4608,13 +4108,10 @@
         </is>
       </c>
       <c r="D167" t="n">
-        <v>0</v>
+        <v>49209.08</v>
       </c>
       <c r="E167" t="n">
-        <v>49209.08</v>
-      </c>
-      <c r="F167" t="n">
-        <v>165</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168">
@@ -4634,13 +4131,10 @@
         </is>
       </c>
       <c r="D168" t="n">
-        <v>0</v>
+        <v>49943.9</v>
       </c>
       <c r="E168" t="n">
-        <v>49943.9</v>
-      </c>
-      <c r="F168" t="n">
-        <v>166</v>
+        <v>0</v>
       </c>
     </row>
     <row r="169">
@@ -4660,13 +4154,10 @@
         </is>
       </c>
       <c r="D169" t="n">
-        <v>0</v>
+        <v>52448.89</v>
       </c>
       <c r="E169" t="n">
-        <v>52448.89</v>
-      </c>
-      <c r="F169" t="n">
-        <v>167</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170">
@@ -4686,13 +4177,10 @@
         </is>
       </c>
       <c r="D170" t="n">
-        <v>0</v>
+        <v>53499.96</v>
       </c>
       <c r="E170" t="n">
-        <v>53499.96</v>
-      </c>
-      <c r="F170" t="n">
-        <v>168</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171">
@@ -4712,13 +4200,10 @@
         </is>
       </c>
       <c r="D171" t="n">
-        <v>0</v>
+        <v>54896.4</v>
       </c>
       <c r="E171" t="n">
-        <v>54896.4</v>
-      </c>
-      <c r="F171" t="n">
-        <v>169</v>
+        <v>0</v>
       </c>
     </row>
     <row r="172">
@@ -4738,13 +4223,10 @@
         </is>
       </c>
       <c r="D172" t="n">
-        <v>0</v>
+        <v>55262.38</v>
       </c>
       <c r="E172" t="n">
-        <v>55262.38</v>
-      </c>
-      <c r="F172" t="n">
-        <v>170</v>
+        <v>0</v>
       </c>
     </row>
     <row r="173">
@@ -4764,13 +4246,10 @@
         </is>
       </c>
       <c r="D173" t="n">
-        <v>0</v>
+        <v>55458.8</v>
       </c>
       <c r="E173" t="n">
-        <v>55458.8</v>
-      </c>
-      <c r="F173" t="n">
-        <v>171</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174">
@@ -4790,13 +4269,10 @@
         </is>
       </c>
       <c r="D174" t="n">
-        <v>0</v>
+        <v>56050.43</v>
       </c>
       <c r="E174" t="n">
-        <v>56050.43</v>
-      </c>
-      <c r="F174" t="n">
-        <v>172</v>
+        <v>0</v>
       </c>
     </row>
     <row r="175">
@@ -4816,13 +4292,10 @@
         </is>
       </c>
       <c r="D175" t="n">
-        <v>0</v>
+        <v>57882.83</v>
       </c>
       <c r="E175" t="n">
-        <v>57882.83</v>
-      </c>
-      <c r="F175" t="n">
-        <v>173</v>
+        <v>0</v>
       </c>
     </row>
     <row r="176">
@@ -4842,13 +4315,10 @@
         </is>
       </c>
       <c r="D176" t="n">
-        <v>0</v>
+        <v>61691.18</v>
       </c>
       <c r="E176" t="n">
-        <v>61691.18</v>
-      </c>
-      <c r="F176" t="n">
-        <v>174</v>
+        <v>0</v>
       </c>
     </row>
     <row r="177">
@@ -4868,13 +4338,10 @@
         </is>
       </c>
       <c r="D177" t="n">
-        <v>0</v>
+        <v>62423.35</v>
       </c>
       <c r="E177" t="n">
-        <v>62423.35</v>
-      </c>
-      <c r="F177" t="n">
-        <v>175</v>
+        <v>0</v>
       </c>
     </row>
     <row r="178">
@@ -4894,13 +4361,10 @@
         </is>
       </c>
       <c r="D178" t="n">
-        <v>0</v>
+        <v>64408.94</v>
       </c>
       <c r="E178" t="n">
-        <v>64408.94</v>
-      </c>
-      <c r="F178" t="n">
-        <v>176</v>
+        <v>0</v>
       </c>
     </row>
     <row r="179">
@@ -4920,13 +4384,10 @@
         </is>
       </c>
       <c r="D179" t="n">
-        <v>0</v>
+        <v>64894.28</v>
       </c>
       <c r="E179" t="n">
-        <v>64894.28</v>
-      </c>
-      <c r="F179" t="n">
-        <v>177</v>
+        <v>0</v>
       </c>
     </row>
     <row r="180">
@@ -4946,13 +4407,10 @@
         </is>
       </c>
       <c r="D180" t="n">
-        <v>0</v>
+        <v>65380.34</v>
       </c>
       <c r="E180" t="n">
-        <v>65380.34</v>
-      </c>
-      <c r="F180" t="n">
-        <v>178</v>
+        <v>0</v>
       </c>
     </row>
     <row r="181">
@@ -4972,13 +4430,10 @@
         </is>
       </c>
       <c r="D181" t="n">
-        <v>0</v>
+        <v>66114</v>
       </c>
       <c r="E181" t="n">
-        <v>66114</v>
-      </c>
-      <c r="F181" t="n">
-        <v>179</v>
+        <v>0</v>
       </c>
     </row>
     <row r="182">
@@ -4998,13 +4453,10 @@
         </is>
       </c>
       <c r="D182" t="n">
-        <v>0</v>
+        <v>67081.73</v>
       </c>
       <c r="E182" t="n">
-        <v>67081.73</v>
-      </c>
-      <c r="F182" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="183">
@@ -5024,13 +4476,10 @@
         </is>
       </c>
       <c r="D183" t="n">
-        <v>0</v>
+        <v>67383.32000000001</v>
       </c>
       <c r="E183" t="n">
-        <v>67383.32000000001</v>
-      </c>
-      <c r="F183" t="n">
-        <v>181</v>
+        <v>0</v>
       </c>
     </row>
     <row r="184">
@@ -5050,13 +4499,10 @@
         </is>
       </c>
       <c r="D184" t="n">
-        <v>0</v>
+        <v>67992.25</v>
       </c>
       <c r="E184" t="n">
-        <v>67992.25</v>
-      </c>
-      <c r="F184" t="n">
-        <v>182</v>
+        <v>0</v>
       </c>
     </row>
     <row r="185">
@@ -5076,13 +4522,10 @@
         </is>
       </c>
       <c r="D185" t="n">
-        <v>0</v>
+        <v>68000</v>
       </c>
       <c r="E185" t="n">
-        <v>68000</v>
-      </c>
-      <c r="F185" t="n">
-        <v>183</v>
+        <v>0</v>
       </c>
     </row>
     <row r="186">
@@ -5102,13 +4545,10 @@
         </is>
       </c>
       <c r="D186" t="n">
-        <v>0</v>
+        <v>68890.47</v>
       </c>
       <c r="E186" t="n">
-        <v>68890.47</v>
-      </c>
-      <c r="F186" t="n">
-        <v>184</v>
+        <v>0</v>
       </c>
     </row>
     <row r="187">
@@ -5128,13 +4568,10 @@
         </is>
       </c>
       <c r="D187" t="n">
-        <v>0</v>
+        <v>71889.38</v>
       </c>
       <c r="E187" t="n">
-        <v>71889.38</v>
-      </c>
-      <c r="F187" t="n">
-        <v>185</v>
+        <v>0</v>
       </c>
     </row>
     <row r="188">
@@ -5154,13 +4591,10 @@
         </is>
       </c>
       <c r="D188" t="n">
-        <v>0</v>
+        <v>72758.11</v>
       </c>
       <c r="E188" t="n">
-        <v>72758.11</v>
-      </c>
-      <c r="F188" t="n">
-        <v>186</v>
+        <v>0</v>
       </c>
     </row>
     <row r="189">
@@ -5180,13 +4614,10 @@
         </is>
       </c>
       <c r="D189" t="n">
-        <v>0</v>
+        <v>73125</v>
       </c>
       <c r="E189" t="n">
-        <v>73125</v>
-      </c>
-      <c r="F189" t="n">
-        <v>187</v>
+        <v>0</v>
       </c>
     </row>
     <row r="190">
@@ -5206,13 +4637,10 @@
         </is>
       </c>
       <c r="D190" t="n">
-        <v>0</v>
+        <v>74344.37</v>
       </c>
       <c r="E190" t="n">
-        <v>74344.37</v>
-      </c>
-      <c r="F190" t="n">
-        <v>188</v>
+        <v>0</v>
       </c>
     </row>
     <row r="191">
@@ -5232,13 +4660,10 @@
         </is>
       </c>
       <c r="D191" t="n">
-        <v>0</v>
+        <v>77130</v>
       </c>
       <c r="E191" t="n">
-        <v>77130</v>
-      </c>
-      <c r="F191" t="n">
-        <v>189</v>
+        <v>0</v>
       </c>
     </row>
     <row r="192">
@@ -5258,13 +4683,10 @@
         </is>
       </c>
       <c r="D192" t="n">
-        <v>0</v>
+        <v>77634.36</v>
       </c>
       <c r="E192" t="n">
-        <v>77634.36</v>
-      </c>
-      <c r="F192" t="n">
-        <v>190</v>
+        <v>0</v>
       </c>
     </row>
     <row r="193">
@@ -5284,13 +4706,10 @@
         </is>
       </c>
       <c r="D193" t="n">
-        <v>0</v>
+        <v>77774.58</v>
       </c>
       <c r="E193" t="n">
-        <v>77774.58</v>
-      </c>
-      <c r="F193" t="n">
-        <v>191</v>
+        <v>0</v>
       </c>
     </row>
     <row r="194">
@@ -5310,13 +4729,10 @@
         </is>
       </c>
       <c r="D194" t="n">
-        <v>0</v>
+        <v>78625.14999999999</v>
       </c>
       <c r="E194" t="n">
-        <v>78625.14999999999</v>
-      </c>
-      <c r="F194" t="n">
-        <v>192</v>
+        <v>0</v>
       </c>
     </row>
     <row r="195">
@@ -5336,13 +4752,10 @@
         </is>
       </c>
       <c r="D195" t="n">
-        <v>0</v>
+        <v>81179.48</v>
       </c>
       <c r="E195" t="n">
-        <v>81179.48</v>
-      </c>
-      <c r="F195" t="n">
-        <v>193</v>
+        <v>0</v>
       </c>
     </row>
     <row r="196">
@@ -5362,13 +4775,10 @@
         </is>
       </c>
       <c r="D196" t="n">
-        <v>0</v>
+        <v>81784.27</v>
       </c>
       <c r="E196" t="n">
-        <v>81784.27</v>
-      </c>
-      <c r="F196" t="n">
-        <v>194</v>
+        <v>0</v>
       </c>
     </row>
     <row r="197">
@@ -5388,13 +4798,10 @@
         </is>
       </c>
       <c r="D197" t="n">
-        <v>0</v>
+        <v>83381.17</v>
       </c>
       <c r="E197" t="n">
-        <v>83381.17</v>
-      </c>
-      <c r="F197" t="n">
-        <v>195</v>
+        <v>0</v>
       </c>
     </row>
     <row r="198">
@@ -5414,13 +4821,10 @@
         </is>
       </c>
       <c r="D198" t="n">
-        <v>0</v>
+        <v>83392.02</v>
       </c>
       <c r="E198" t="n">
-        <v>83392.02</v>
-      </c>
-      <c r="F198" t="n">
-        <v>196</v>
+        <v>0</v>
       </c>
     </row>
     <row r="199">
@@ -5440,13 +4844,10 @@
         </is>
       </c>
       <c r="D199" t="n">
-        <v>0</v>
+        <v>83818.21000000001</v>
       </c>
       <c r="E199" t="n">
-        <v>83818.21000000001</v>
-      </c>
-      <c r="F199" t="n">
-        <v>197</v>
+        <v>0</v>
       </c>
     </row>
     <row r="200">
@@ -5466,13 +4867,10 @@
         </is>
       </c>
       <c r="D200" t="n">
-        <v>0</v>
+        <v>89655.37</v>
       </c>
       <c r="E200" t="n">
-        <v>89655.37</v>
-      </c>
-      <c r="F200" t="n">
-        <v>198</v>
+        <v>0</v>
       </c>
     </row>
     <row r="201">
@@ -5492,13 +4890,10 @@
         </is>
       </c>
       <c r="D201" t="n">
-        <v>0</v>
+        <v>90990.42999999999</v>
       </c>
       <c r="E201" t="n">
-        <v>90990.42999999999</v>
-      </c>
-      <c r="F201" t="n">
-        <v>199</v>
+        <v>0</v>
       </c>
     </row>
     <row r="202">
@@ -5518,13 +4913,10 @@
         </is>
       </c>
       <c r="D202" t="n">
-        <v>0</v>
+        <v>93399.52</v>
       </c>
       <c r="E202" t="n">
-        <v>93399.52</v>
-      </c>
-      <c r="F202" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="203">
@@ -5544,13 +4936,10 @@
         </is>
       </c>
       <c r="D203" t="n">
-        <v>0</v>
+        <v>93523.19</v>
       </c>
       <c r="E203" t="n">
-        <v>93523.19</v>
-      </c>
-      <c r="F203" t="n">
-        <v>201</v>
+        <v>0</v>
       </c>
     </row>
     <row r="204">
@@ -5570,13 +4959,10 @@
         </is>
       </c>
       <c r="D204" t="n">
-        <v>0</v>
+        <v>95590.62</v>
       </c>
       <c r="E204" t="n">
-        <v>95590.62</v>
-      </c>
-      <c r="F204" t="n">
-        <v>202</v>
+        <v>0</v>
       </c>
     </row>
     <row r="205">
@@ -5596,13 +4982,10 @@
         </is>
       </c>
       <c r="D205" t="n">
-        <v>0</v>
+        <v>100200.01</v>
       </c>
       <c r="E205" t="n">
-        <v>100200.01</v>
-      </c>
-      <c r="F205" t="n">
-        <v>203</v>
+        <v>0</v>
       </c>
     </row>
     <row r="206">
@@ -5622,13 +5005,10 @@
         </is>
       </c>
       <c r="D206" t="n">
-        <v>0</v>
+        <v>102978.96</v>
       </c>
       <c r="E206" t="n">
-        <v>102978.96</v>
-      </c>
-      <c r="F206" t="n">
-        <v>204</v>
+        <v>0</v>
       </c>
     </row>
     <row r="207">
@@ -5648,13 +5028,10 @@
         </is>
       </c>
       <c r="D207" t="n">
-        <v>0</v>
+        <v>103296.78</v>
       </c>
       <c r="E207" t="n">
-        <v>103296.78</v>
-      </c>
-      <c r="F207" t="n">
-        <v>205</v>
+        <v>0</v>
       </c>
     </row>
     <row r="208">
@@ -5674,13 +5051,10 @@
         </is>
       </c>
       <c r="D208" t="n">
-        <v>0</v>
+        <v>111687.2</v>
       </c>
       <c r="E208" t="n">
-        <v>111687.2</v>
-      </c>
-      <c r="F208" t="n">
-        <v>206</v>
+        <v>0</v>
       </c>
     </row>
     <row r="209">
@@ -5700,13 +5074,10 @@
         </is>
       </c>
       <c r="D209" t="n">
-        <v>0</v>
+        <v>111708.63</v>
       </c>
       <c r="E209" t="n">
-        <v>111708.63</v>
-      </c>
-      <c r="F209" t="n">
-        <v>207</v>
+        <v>0</v>
       </c>
     </row>
     <row r="210">
@@ -5726,13 +5097,10 @@
         </is>
       </c>
       <c r="D210" t="n">
-        <v>0</v>
+        <v>119019.85</v>
       </c>
       <c r="E210" t="n">
-        <v>119019.85</v>
-      </c>
-      <c r="F210" t="n">
-        <v>208</v>
+        <v>0</v>
       </c>
     </row>
     <row r="211">
@@ -5752,13 +5120,10 @@
         </is>
       </c>
       <c r="D211" t="n">
-        <v>0</v>
+        <v>119974.79</v>
       </c>
       <c r="E211" t="n">
-        <v>119974.79</v>
-      </c>
-      <c r="F211" t="n">
-        <v>209</v>
+        <v>0</v>
       </c>
     </row>
     <row r="212">
@@ -5778,13 +5143,10 @@
         </is>
       </c>
       <c r="D212" t="n">
-        <v>0</v>
+        <v>120577.79</v>
       </c>
       <c r="E212" t="n">
-        <v>120577.79</v>
-      </c>
-      <c r="F212" t="n">
-        <v>210</v>
+        <v>0</v>
       </c>
     </row>
     <row r="213">
@@ -5804,13 +5166,10 @@
         </is>
       </c>
       <c r="D213" t="n">
-        <v>0</v>
+        <v>121994.8</v>
       </c>
       <c r="E213" t="n">
-        <v>121994.8</v>
-      </c>
-      <c r="F213" t="n">
-        <v>211</v>
+        <v>0</v>
       </c>
     </row>
     <row r="214">
@@ -5830,13 +5189,10 @@
         </is>
       </c>
       <c r="D214" t="n">
-        <v>0</v>
+        <v>133212.15</v>
       </c>
       <c r="E214" t="n">
-        <v>133212.15</v>
-      </c>
-      <c r="F214" t="n">
-        <v>212</v>
+        <v>0</v>
       </c>
     </row>
     <row r="215">
@@ -5856,13 +5212,10 @@
         </is>
       </c>
       <c r="D215" t="n">
-        <v>0</v>
+        <v>136711.62</v>
       </c>
       <c r="E215" t="n">
-        <v>136711.62</v>
-      </c>
-      <c r="F215" t="n">
-        <v>213</v>
+        <v>0</v>
       </c>
     </row>
     <row r="216">
@@ -5882,13 +5235,10 @@
         </is>
       </c>
       <c r="D216" t="n">
-        <v>0</v>
+        <v>138110.42</v>
       </c>
       <c r="E216" t="n">
-        <v>138110.42</v>
-      </c>
-      <c r="F216" t="n">
-        <v>214</v>
+        <v>0</v>
       </c>
     </row>
     <row r="217">
@@ -5908,13 +5258,10 @@
         </is>
       </c>
       <c r="D217" t="n">
-        <v>0</v>
+        <v>138371.09</v>
       </c>
       <c r="E217" t="n">
-        <v>138371.09</v>
-      </c>
-      <c r="F217" t="n">
-        <v>215</v>
+        <v>0</v>
       </c>
     </row>
     <row r="218">
@@ -5934,13 +5281,10 @@
         </is>
       </c>
       <c r="D218" t="n">
-        <v>0</v>
+        <v>138830.65</v>
       </c>
       <c r="E218" t="n">
-        <v>138830.65</v>
-      </c>
-      <c r="F218" t="n">
-        <v>216</v>
+        <v>0</v>
       </c>
     </row>
     <row r="219">
@@ -5960,13 +5304,10 @@
         </is>
       </c>
       <c r="D219" t="n">
-        <v>0</v>
+        <v>140562.21</v>
       </c>
       <c r="E219" t="n">
-        <v>140562.21</v>
-      </c>
-      <c r="F219" t="n">
-        <v>217</v>
+        <v>0</v>
       </c>
     </row>
     <row r="220">
@@ -5986,13 +5327,10 @@
         </is>
       </c>
       <c r="D220" t="n">
-        <v>0</v>
+        <v>144960.81</v>
       </c>
       <c r="E220" t="n">
-        <v>144960.81</v>
-      </c>
-      <c r="F220" t="n">
-        <v>218</v>
+        <v>0</v>
       </c>
     </row>
     <row r="221">
@@ -6012,13 +5350,10 @@
         </is>
       </c>
       <c r="D221" t="n">
-        <v>0</v>
+        <v>148942.4</v>
       </c>
       <c r="E221" t="n">
-        <v>148942.4</v>
-      </c>
-      <c r="F221" t="n">
-        <v>219</v>
+        <v>0</v>
       </c>
     </row>
     <row r="222">
@@ -6038,13 +5373,10 @@
         </is>
       </c>
       <c r="D222" t="n">
-        <v>0</v>
+        <v>154696.07</v>
       </c>
       <c r="E222" t="n">
-        <v>154696.07</v>
-      </c>
-      <c r="F222" t="n">
-        <v>220</v>
+        <v>0</v>
       </c>
     </row>
     <row r="223">
@@ -6064,13 +5396,10 @@
         </is>
       </c>
       <c r="D223" t="n">
-        <v>0</v>
+        <v>158585</v>
       </c>
       <c r="E223" t="n">
-        <v>158585</v>
-      </c>
-      <c r="F223" t="n">
-        <v>221</v>
+        <v>0</v>
       </c>
     </row>
     <row r="224">
@@ -6090,13 +5419,10 @@
         </is>
       </c>
       <c r="D224" t="n">
-        <v>0</v>
+        <v>159368.08</v>
       </c>
       <c r="E224" t="n">
-        <v>159368.08</v>
-      </c>
-      <c r="F224" t="n">
-        <v>222</v>
+        <v>0</v>
       </c>
     </row>
     <row r="225">
@@ -6116,13 +5442,10 @@
         </is>
       </c>
       <c r="D225" t="n">
-        <v>0</v>
+        <v>161552.59</v>
       </c>
       <c r="E225" t="n">
-        <v>161552.59</v>
-      </c>
-      <c r="F225" t="n">
-        <v>223</v>
+        <v>0</v>
       </c>
     </row>
     <row r="226">
@@ -6142,13 +5465,10 @@
         </is>
       </c>
       <c r="D226" t="n">
-        <v>0</v>
+        <v>164501.66</v>
       </c>
       <c r="E226" t="n">
-        <v>164501.66</v>
-      </c>
-      <c r="F226" t="n">
-        <v>224</v>
+        <v>0</v>
       </c>
     </row>
     <row r="227">
@@ -6168,13 +5488,10 @@
         </is>
       </c>
       <c r="D227" t="n">
-        <v>0</v>
+        <v>164579.28</v>
       </c>
       <c r="E227" t="n">
-        <v>164579.28</v>
-      </c>
-      <c r="F227" t="n">
-        <v>225</v>
+        <v>0</v>
       </c>
     </row>
     <row r="228">
@@ -6194,13 +5511,10 @@
         </is>
       </c>
       <c r="D228" t="n">
-        <v>0</v>
+        <v>166268.09</v>
       </c>
       <c r="E228" t="n">
-        <v>166268.09</v>
-      </c>
-      <c r="F228" t="n">
-        <v>226</v>
+        <v>0</v>
       </c>
     </row>
     <row r="229">
@@ -6220,13 +5534,10 @@
         </is>
       </c>
       <c r="D229" t="n">
-        <v>0</v>
+        <v>174263.6</v>
       </c>
       <c r="E229" t="n">
-        <v>174263.6</v>
-      </c>
-      <c r="F229" t="n">
-        <v>227</v>
+        <v>0</v>
       </c>
     </row>
     <row r="230">
@@ -6246,13 +5557,10 @@
         </is>
       </c>
       <c r="D230" t="n">
-        <v>0</v>
+        <v>176808.88</v>
       </c>
       <c r="E230" t="n">
-        <v>176808.88</v>
-      </c>
-      <c r="F230" t="n">
-        <v>228</v>
+        <v>0</v>
       </c>
     </row>
     <row r="231">
@@ -6272,13 +5580,10 @@
         </is>
       </c>
       <c r="D231" t="n">
-        <v>0</v>
+        <v>181760.83</v>
       </c>
       <c r="E231" t="n">
-        <v>181760.83</v>
-      </c>
-      <c r="F231" t="n">
-        <v>229</v>
+        <v>0</v>
       </c>
     </row>
     <row r="232">
@@ -6298,13 +5603,10 @@
         </is>
       </c>
       <c r="D232" t="n">
-        <v>0</v>
+        <v>184692.76</v>
       </c>
       <c r="E232" t="n">
-        <v>184692.76</v>
-      </c>
-      <c r="F232" t="n">
-        <v>230</v>
+        <v>0</v>
       </c>
     </row>
     <row r="233">
@@ -6324,13 +5626,10 @@
         </is>
       </c>
       <c r="D233" t="n">
-        <v>0</v>
+        <v>188743.76</v>
       </c>
       <c r="E233" t="n">
-        <v>188743.76</v>
-      </c>
-      <c r="F233" t="n">
-        <v>231</v>
+        <v>0</v>
       </c>
     </row>
     <row r="234">
@@ -6350,13 +5649,10 @@
         </is>
       </c>
       <c r="D234" t="n">
-        <v>0</v>
+        <v>199413.63</v>
       </c>
       <c r="E234" t="n">
-        <v>199413.63</v>
-      </c>
-      <c r="F234" t="n">
-        <v>232</v>
+        <v>0</v>
       </c>
     </row>
     <row r="235">
@@ -6376,13 +5672,10 @@
         </is>
       </c>
       <c r="D235" t="n">
-        <v>0</v>
+        <v>201207.84</v>
       </c>
       <c r="E235" t="n">
-        <v>201207.84</v>
-      </c>
-      <c r="F235" t="n">
-        <v>233</v>
+        <v>0</v>
       </c>
     </row>
     <row r="236">
@@ -6402,13 +5695,10 @@
         </is>
       </c>
       <c r="D236" t="n">
-        <v>0</v>
+        <v>204337.44</v>
       </c>
       <c r="E236" t="n">
-        <v>204337.44</v>
-      </c>
-      <c r="F236" t="n">
-        <v>234</v>
+        <v>0</v>
       </c>
     </row>
     <row r="237">
@@ -6428,13 +5718,10 @@
         </is>
       </c>
       <c r="D237" t="n">
-        <v>0</v>
+        <v>207747.5</v>
       </c>
       <c r="E237" t="n">
-        <v>207747.5</v>
-      </c>
-      <c r="F237" t="n">
-        <v>235</v>
+        <v>0</v>
       </c>
     </row>
     <row r="238">
@@ -6454,13 +5741,10 @@
         </is>
       </c>
       <c r="D238" t="n">
-        <v>0</v>
+        <v>208021.84</v>
       </c>
       <c r="E238" t="n">
-        <v>208021.84</v>
-      </c>
-      <c r="F238" t="n">
-        <v>236</v>
+        <v>0</v>
       </c>
     </row>
     <row r="239">
@@ -6480,13 +5764,10 @@
         </is>
       </c>
       <c r="D239" t="n">
-        <v>0</v>
+        <v>215550.42</v>
       </c>
       <c r="E239" t="n">
-        <v>215550.42</v>
-      </c>
-      <c r="F239" t="n">
-        <v>237</v>
+        <v>0</v>
       </c>
     </row>
     <row r="240">
@@ -6506,13 +5787,10 @@
         </is>
       </c>
       <c r="D240" t="n">
-        <v>0</v>
+        <v>218888.75</v>
       </c>
       <c r="E240" t="n">
-        <v>218888.75</v>
-      </c>
-      <c r="F240" t="n">
-        <v>238</v>
+        <v>0</v>
       </c>
     </row>
     <row r="241">
@@ -6532,13 +5810,10 @@
         </is>
       </c>
       <c r="D241" t="n">
-        <v>0</v>
+        <v>227974.05</v>
       </c>
       <c r="E241" t="n">
-        <v>227974.05</v>
-      </c>
-      <c r="F241" t="n">
-        <v>239</v>
+        <v>0</v>
       </c>
     </row>
     <row r="242">
@@ -6558,13 +5833,10 @@
         </is>
       </c>
       <c r="D242" t="n">
-        <v>0</v>
+        <v>230901.72</v>
       </c>
       <c r="E242" t="n">
-        <v>230901.72</v>
-      </c>
-      <c r="F242" t="n">
-        <v>240</v>
+        <v>0</v>
       </c>
     </row>
     <row r="243">
@@ -6584,13 +5856,10 @@
         </is>
       </c>
       <c r="D243" t="n">
-        <v>0</v>
+        <v>248569.72</v>
       </c>
       <c r="E243" t="n">
-        <v>248569.72</v>
-      </c>
-      <c r="F243" t="n">
-        <v>241</v>
+        <v>0</v>
       </c>
     </row>
     <row r="244">
@@ -6610,13 +5879,10 @@
         </is>
       </c>
       <c r="D244" t="n">
-        <v>0</v>
+        <v>260688.69</v>
       </c>
       <c r="E244" t="n">
-        <v>260688.69</v>
-      </c>
-      <c r="F244" t="n">
-        <v>242</v>
+        <v>0</v>
       </c>
     </row>
     <row r="245">
@@ -6636,13 +5902,10 @@
         </is>
       </c>
       <c r="D245" t="n">
-        <v>0</v>
+        <v>345041.4</v>
       </c>
       <c r="E245" t="n">
-        <v>345041.4</v>
-      </c>
-      <c r="F245" t="n">
-        <v>243</v>
+        <v>0</v>
       </c>
     </row>
     <row r="246">
@@ -6662,13 +5925,10 @@
         </is>
       </c>
       <c r="D246" t="n">
-        <v>0</v>
+        <v>367789.8</v>
       </c>
       <c r="E246" t="n">
-        <v>367789.8</v>
-      </c>
-      <c r="F246" t="n">
-        <v>244</v>
+        <v>0</v>
       </c>
     </row>
     <row r="247">
@@ -6688,13 +5948,10 @@
         </is>
       </c>
       <c r="D247" t="n">
-        <v>0</v>
+        <v>371760.23</v>
       </c>
       <c r="E247" t="n">
-        <v>371760.23</v>
-      </c>
-      <c r="F247" t="n">
-        <v>245</v>
+        <v>0</v>
       </c>
     </row>
     <row r="248">
@@ -6714,13 +5971,10 @@
         </is>
       </c>
       <c r="D248" t="n">
-        <v>0</v>
+        <v>424560.61</v>
       </c>
       <c r="E248" t="n">
-        <v>424560.61</v>
-      </c>
-      <c r="F248" t="n">
-        <v>246</v>
+        <v>0</v>
       </c>
     </row>
     <row r="249">
@@ -6740,13 +5994,10 @@
         </is>
       </c>
       <c r="D249" t="n">
-        <v>0</v>
+        <v>434801.08</v>
       </c>
       <c r="E249" t="n">
-        <v>434801.08</v>
-      </c>
-      <c r="F249" t="n">
-        <v>247</v>
+        <v>0</v>
       </c>
     </row>
     <row r="250">
@@ -6766,13 +6017,10 @@
         </is>
       </c>
       <c r="D250" t="n">
-        <v>0</v>
+        <v>454685.4</v>
       </c>
       <c r="E250" t="n">
-        <v>454685.4</v>
-      </c>
-      <c r="F250" t="n">
-        <v>248</v>
+        <v>0</v>
       </c>
     </row>
     <row r="251">
@@ -6792,13 +6040,10 @@
         </is>
       </c>
       <c r="D251" t="n">
-        <v>0</v>
+        <v>456234.82</v>
       </c>
       <c r="E251" t="n">
-        <v>456234.82</v>
-      </c>
-      <c r="F251" t="n">
-        <v>249</v>
+        <v>0</v>
       </c>
     </row>
     <row r="252">
@@ -6818,13 +6063,10 @@
         </is>
       </c>
       <c r="D252" t="n">
-        <v>0</v>
+        <v>466574.58</v>
       </c>
       <c r="E252" t="n">
-        <v>466574.58</v>
-      </c>
-      <c r="F252" t="n">
-        <v>250</v>
+        <v>0</v>
       </c>
     </row>
     <row r="253">
@@ -6844,13 +6086,10 @@
         </is>
       </c>
       <c r="D253" t="n">
-        <v>0</v>
+        <v>572295.98</v>
       </c>
       <c r="E253" t="n">
-        <v>572295.98</v>
-      </c>
-      <c r="F253" t="n">
-        <v>251</v>
+        <v>0</v>
       </c>
     </row>
     <row r="254">
@@ -6870,13 +6109,10 @@
         </is>
       </c>
       <c r="D254" t="n">
-        <v>0</v>
+        <v>579173.17</v>
       </c>
       <c r="E254" t="n">
-        <v>579173.17</v>
-      </c>
-      <c r="F254" t="n">
-        <v>252</v>
+        <v>0</v>
       </c>
     </row>
     <row r="255">
@@ -6896,13 +6132,10 @@
         </is>
       </c>
       <c r="D255" t="n">
-        <v>0</v>
+        <v>584807.72</v>
       </c>
       <c r="E255" t="n">
-        <v>584807.72</v>
-      </c>
-      <c r="F255" t="n">
-        <v>253</v>
+        <v>0</v>
       </c>
     </row>
     <row r="256">
@@ -6922,13 +6155,10 @@
         </is>
       </c>
       <c r="D256" t="n">
-        <v>0</v>
+        <v>667087.0699999999</v>
       </c>
       <c r="E256" t="n">
-        <v>667087.0699999999</v>
-      </c>
-      <c r="F256" t="n">
-        <v>254</v>
+        <v>0</v>
       </c>
     </row>
     <row r="257">
@@ -6948,13 +6178,10 @@
         </is>
       </c>
       <c r="D257" t="n">
-        <v>0</v>
+        <v>668418.3100000001</v>
       </c>
       <c r="E257" t="n">
-        <v>668418.3100000001</v>
-      </c>
-      <c r="F257" t="n">
-        <v>255</v>
+        <v>0</v>
       </c>
     </row>
     <row r="258">
@@ -6974,13 +6201,10 @@
         </is>
       </c>
       <c r="D258" t="n">
-        <v>0</v>
+        <v>699581.9</v>
       </c>
       <c r="E258" t="n">
-        <v>699581.9</v>
-      </c>
-      <c r="F258" t="n">
-        <v>256</v>
+        <v>0</v>
       </c>
     </row>
     <row r="259">
@@ -7000,13 +6224,10 @@
         </is>
       </c>
       <c r="D259" t="n">
-        <v>0</v>
+        <v>763280.25</v>
       </c>
       <c r="E259" t="n">
-        <v>763280.25</v>
-      </c>
-      <c r="F259" t="n">
-        <v>257</v>
+        <v>0</v>
       </c>
     </row>
     <row r="260">
@@ -7022,13 +6243,10 @@
       </c>
       <c r="C260" t="inlineStr"/>
       <c r="D260" t="n">
-        <v>0</v>
+        <v>839473.1800000001</v>
       </c>
       <c r="E260" t="n">
-        <v>839473.1800000001</v>
-      </c>
-      <c r="F260" t="n">
-        <v>258</v>
+        <v>0</v>
       </c>
     </row>
     <row r="261">
@@ -7048,13 +6266,10 @@
         </is>
       </c>
       <c r="D261" t="n">
-        <v>0</v>
+        <v>857151.04</v>
       </c>
       <c r="E261" t="n">
-        <v>857151.04</v>
-      </c>
-      <c r="F261" t="n">
-        <v>259</v>
+        <v>0</v>
       </c>
     </row>
     <row r="262">
@@ -7074,13 +6289,10 @@
         </is>
       </c>
       <c r="D262" t="n">
-        <v>0</v>
+        <v>1053305.1</v>
       </c>
       <c r="E262" t="n">
-        <v>1053305.1</v>
-      </c>
-      <c r="F262" t="n">
-        <v>260</v>
+        <v>0</v>
       </c>
     </row>
     <row r="263">
@@ -7100,13 +6312,10 @@
         </is>
       </c>
       <c r="D263" t="n">
-        <v>0</v>
+        <v>1142040.69</v>
       </c>
       <c r="E263" t="n">
-        <v>1142040.69</v>
-      </c>
-      <c r="F263" t="n">
-        <v>261</v>
+        <v>0</v>
       </c>
     </row>
     <row r="264">
@@ -7126,13 +6335,10 @@
         </is>
       </c>
       <c r="D264" t="n">
-        <v>0</v>
+        <v>1169480.67</v>
       </c>
       <c r="E264" t="n">
-        <v>1169480.67</v>
-      </c>
-      <c r="F264" t="n">
-        <v>262</v>
+        <v>0</v>
       </c>
     </row>
     <row r="265">
@@ -7152,13 +6358,10 @@
         </is>
       </c>
       <c r="D265" t="n">
-        <v>0</v>
+        <v>1308547.9</v>
       </c>
       <c r="E265" t="n">
-        <v>1308547.9</v>
-      </c>
-      <c r="F265" t="n">
-        <v>263</v>
+        <v>0</v>
       </c>
     </row>
     <row r="266">
@@ -7178,13 +6381,10 @@
         </is>
       </c>
       <c r="D266" t="n">
-        <v>0</v>
+        <v>1458986.98</v>
       </c>
       <c r="E266" t="n">
-        <v>1458986.98</v>
-      </c>
-      <c r="F266" t="n">
-        <v>264</v>
+        <v>0</v>
       </c>
     </row>
     <row r="267">
@@ -7204,13 +6404,10 @@
         </is>
       </c>
       <c r="D267" t="n">
-        <v>0</v>
+        <v>1845788.21</v>
       </c>
       <c r="E267" t="n">
-        <v>1845788.21</v>
-      </c>
-      <c r="F267" t="n">
-        <v>265</v>
+        <v>0</v>
       </c>
     </row>
     <row r="268">
@@ -7230,13 +6427,10 @@
         </is>
       </c>
       <c r="D268" t="n">
-        <v>0</v>
+        <v>2265124.13</v>
       </c>
       <c r="E268" t="n">
-        <v>2265124.13</v>
-      </c>
-      <c r="F268" t="n">
-        <v>266</v>
+        <v>0</v>
       </c>
     </row>
     <row r="269">
@@ -7256,13 +6450,10 @@
         </is>
       </c>
       <c r="D269" t="n">
-        <v>0</v>
+        <v>2398528.29</v>
       </c>
       <c r="E269" t="n">
-        <v>2398528.29</v>
-      </c>
-      <c r="F269" t="n">
-        <v>267</v>
+        <v>0</v>
       </c>
     </row>
     <row r="270">
@@ -7282,13 +6473,10 @@
         </is>
       </c>
       <c r="D270" t="n">
-        <v>0</v>
+        <v>2499098.06</v>
       </c>
       <c r="E270" t="n">
-        <v>2499098.06</v>
-      </c>
-      <c r="F270" t="n">
-        <v>268</v>
+        <v>0</v>
       </c>
     </row>
     <row r="271">
@@ -7304,13 +6492,10 @@
       </c>
       <c r="C271" t="inlineStr"/>
       <c r="D271" t="n">
+        <v>0</v>
+      </c>
+      <c r="E271" t="n">
         <v>120875808.75</v>
-      </c>
-      <c r="E271" t="n">
-        <v>0</v>
-      </c>
-      <c r="F271" t="n">
-        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>